<commit_message>
testing updated for multijump
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="108">
   <si>
     <t>Instructions</t>
   </si>
@@ -2831,6 +2831,9 @@
   </si>
   <si>
     <t>Failed, bug during rerouting 4/16/2018 (LD)</t>
+  </si>
+  <si>
+    <t>Passed 4/17/2018 (LD)</t>
   </si>
   <si>
     <t>Passed 4/16/2018 (LD)</t>
@@ -4007,9 +4010,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="91" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="91" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G37" sqref="G37"/>
+      <selection pane="topRight" activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -7469,7 +7472,7 @@
       <c r="E30" s="27"/>
       <c r="F30" s="27"/>
       <c r="G30" s="27" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H30" s="27"/>
       <c r="I30" s="25"/>
@@ -8496,7 +8499,7 @@
         <v>72</v>
       </c>
       <c r="G31" s="27" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" spans="1:1025" ht="46.5" x14ac:dyDescent="0.35">
@@ -8505,7 +8508,7 @@
         <v>73</v>
       </c>
       <c r="G32" s="27" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="33" spans="1:1025" ht="31" x14ac:dyDescent="0.35">
@@ -8514,7 +8517,7 @@
         <v>74</v>
       </c>
       <c r="G33" s="27" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:1025" ht="46.5" x14ac:dyDescent="0.35">
@@ -8523,7 +8526,7 @@
         <v>75</v>
       </c>
       <c r="G34" s="27" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="35" spans="1:1025" s="26" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
@@ -8537,7 +8540,9 @@
       <c r="D35" s="27"/>
       <c r="E35" s="27"/>
       <c r="F35" s="27"/>
-      <c r="G35" s="27"/>
+      <c r="G35" s="27" t="s">
+        <v>106</v>
+      </c>
       <c r="H35" s="27"/>
       <c r="I35" s="25"/>
       <c r="J35" s="25"/>
@@ -9562,14 +9567,18 @@
       <c r="B36" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="G36" s="27"/>
+      <c r="G36" s="27" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="37" spans="1:1025" ht="31" x14ac:dyDescent="0.35">
       <c r="A37" s="58"/>
       <c r="B37" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="G37" s="27"/>
+      <c r="G37" s="27" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="38" spans="1:1025" s="26" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A38" s="31" t="s">

</xml_diff>

<commit_message>
updated testing for king me and winning
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="108">
   <si>
     <t>Instructions</t>
   </si>
@@ -4010,9 +4010,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="91" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="91" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G36" sqref="G36"/>
+      <selection pane="topRight" activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -9591,7 +9591,9 @@
       <c r="D38" s="27"/>
       <c r="E38" s="27"/>
       <c r="F38" s="27"/>
-      <c r="G38" s="27"/>
+      <c r="G38" s="27" t="s">
+        <v>106</v>
+      </c>
       <c r="H38" s="27"/>
       <c r="I38" s="25"/>
       <c r="J38" s="25"/>
@@ -10622,7 +10624,9 @@
       <c r="D39" s="27"/>
       <c r="E39" s="27"/>
       <c r="F39" s="27"/>
-      <c r="G39" s="27"/>
+      <c r="G39" s="27" t="s">
+        <v>106</v>
+      </c>
       <c r="H39" s="27"/>
       <c r="I39" s="25"/>
       <c r="J39" s="25"/>
@@ -11647,14 +11651,18 @@
       <c r="B40" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="G40" s="27"/>
+      <c r="G40" s="27" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="41" spans="1:1025" ht="31" x14ac:dyDescent="0.35">
       <c r="A41" s="50"/>
       <c r="B41" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="G41" s="27"/>
+      <c r="G41" s="27" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="42" spans="1:1025" s="26" customFormat="1" ht="56" x14ac:dyDescent="0.35">
       <c r="A42" s="28" t="s">

</xml_diff>